<commit_message>
Modification Burndown Chart + avancement Plan de Financement
</commit_message>
<xml_diff>
--- a/Etude Economique/Plan de financement.xlsx
+++ b/Etude Economique/Plan de financement.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Besoins initiaux :</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>Frais hébergement site Web</t>
+  </si>
+  <si>
+    <t>Plan de financement</t>
+  </si>
+  <si>
+    <t>Variation du B.F.R</t>
+  </si>
+  <si>
+    <t>Investissements</t>
   </si>
 </sst>
 </file>
@@ -210,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,10 +228,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -242,13 +247,44 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -283,22 +319,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:C8" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:C8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
   <autoFilter ref="B2:C8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Besoins initiaux :"/>
-    <tableColumn id="2" name="Coûts"/>
+    <tableColumn id="1" name="Besoins initiaux :" dataDxfId="2"/>
+    <tableColumn id="2" name="Coûts" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="E2:F3" totalsRowShown="0">
-  <autoFilter ref="E2:F3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="F2:G3" totalsRowShown="0">
+  <autoFilter ref="F2:G3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Apports :"/>
-    <tableColumn id="2" name="Montant" dataDxfId="0"/>
+    <tableColumn id="1" name="Apports :" dataDxfId="4"/>
+    <tableColumn id="2" name="Montant" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -601,16 +637,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -620,118 +656,166 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="15">
         <v>6000</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="13">
         <v>12000</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="15">
         <v>4076</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="15">
         <v>200</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="15">
         <v>700</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="18">
         <f>SUM(C3:C7)</f>
         <v>11026</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <f>C8</f>
         <v>11026</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <f>Tableau3[Montant]</f>
         <v>12000</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <f>G9</f>
         <v>11026</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="6">
         <f>I9</f>
         <v>12000</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I15" s="14"/>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>2019</v>
+      </c>
+      <c r="D15">
+        <v>2020</v>
+      </c>
+      <c r="E15">
+        <v>2021</v>
+      </c>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="14"/>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2720</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2720</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2720</v>
+      </c>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>